<commit_message>
Opraveno: Chybějící hodnoty nahrazovány nulou.
</commit_message>
<xml_diff>
--- a/data/azyly_2015.xlsx
+++ b/data/azyly_2015.xlsx
@@ -628,9 +628,6 @@
       <c r="E3">
         <v>1821</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
@@ -732,9 +729,6 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
       <c r="G7" t="s">
         <v>8</v>
       </c>
@@ -755,12 +749,6 @@
       <c r="D8">
         <v>53</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
       <c r="G8" t="s">
         <v>8</v>
       </c>
@@ -810,9 +798,6 @@
       <c r="E10">
         <v>313</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
       <c r="G10" t="s">
         <v>8</v>
       </c>
@@ -862,9 +847,6 @@
       <c r="E12">
         <v>12</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
       <c r="G12" t="s">
         <v>8</v>
       </c>
@@ -888,9 +870,6 @@
       <c r="E13">
         <v>204</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
       <c r="G13" t="s">
         <v>8</v>
       </c>
@@ -940,9 +919,6 @@
       <c r="E15">
         <v>353</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
       <c r="G15" t="s">
         <v>8</v>
       </c>
@@ -966,9 +942,6 @@
       <c r="E16">
         <v>2034</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
       <c r="G16" t="s">
         <v>8</v>
       </c>
@@ -992,9 +965,6 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
       <c r="G17" t="s">
         <v>8</v>
       </c>
@@ -1014,12 +984,6 @@
       </c>
       <c r="D18">
         <v>1</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
       </c>
       <c r="G18" t="s">
         <v>8</v>
@@ -1041,12 +1005,6 @@
       <c r="D19">
         <v>36</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
       <c r="G19" t="s">
         <v>8</v>
       </c>
@@ -1069,9 +1027,6 @@
       </c>
       <c r="E20">
         <v>1</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
       </c>
       <c r="G20" t="s">
         <v>8</v>
@@ -1278,9 +1233,6 @@
       <c r="E28">
         <v>16</v>
       </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
       <c r="G28" t="s">
         <v>8</v>
       </c>
@@ -1303,9 +1255,6 @@
       </c>
       <c r="E29">
         <v>1</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
       </c>
       <c r="G29" t="s">
         <v>8</v>
@@ -1382,9 +1331,6 @@
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
       <c r="G32" t="s">
         <v>8</v>
       </c>
@@ -1434,9 +1380,6 @@
       <c r="E34">
         <v>448</v>
       </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
       <c r="G34" t="s">
         <v>8</v>
       </c>
@@ -1538,9 +1481,6 @@
       <c r="E38">
         <v>1194</v>
       </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
       <c r="G38" t="s">
         <v>8</v>
       </c>
@@ -1561,12 +1501,6 @@
       <c r="D39">
         <v>110</v>
       </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
       <c r="G39" t="s">
         <v>8</v>
       </c>
@@ -1587,12 +1521,6 @@
       <c r="D40">
         <v>15</v>
       </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
       <c r="G40" t="s">
         <v>8</v>
       </c>
@@ -1642,9 +1570,6 @@
       <c r="E42">
         <v>1</v>
       </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
       <c r="G42" t="s">
         <v>8</v>
       </c>
@@ -1692,9 +1617,6 @@
         <v>1</v>
       </c>
       <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
         <v>0</v>
       </c>
       <c r="G44" t="s">
@@ -1717,12 +1639,6 @@
       <c r="D45">
         <v>7</v>
       </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
       <c r="G45" t="s">
         <v>8</v>
       </c>
@@ -1772,9 +1688,6 @@
       <c r="E47">
         <v>77</v>
       </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
       <c r="G47" t="s">
         <v>9</v>
       </c>
@@ -1876,9 +1789,6 @@
       <c r="E51">
         <v>1</v>
       </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
       <c r="G51" t="s">
         <v>9</v>
       </c>
@@ -1897,12 +1807,6 @@
         <v>0</v>
       </c>
       <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52">
         <v>0</v>
       </c>
       <c r="G52" t="s">
@@ -1954,9 +1858,6 @@
       <c r="E54">
         <v>31</v>
       </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
       <c r="G54" t="s">
         <v>9</v>
       </c>
@@ -2006,9 +1907,6 @@
       <c r="E56">
         <v>22</v>
       </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
       <c r="G56" t="s">
         <v>9</v>
       </c>
@@ -2032,9 +1930,6 @@
       <c r="E57">
         <v>328</v>
       </c>
-      <c r="F57">
-        <v>0</v>
-      </c>
       <c r="G57" t="s">
         <v>9</v>
       </c>
@@ -2084,9 +1979,6 @@
       <c r="E59">
         <v>0</v>
       </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
       <c r="G59" t="s">
         <v>9</v>
       </c>
@@ -2110,9 +2002,6 @@
       <c r="E60">
         <v>157</v>
       </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
       <c r="G60" t="s">
         <v>9</v>
       </c>
@@ -2136,9 +2025,6 @@
       <c r="E61">
         <v>0</v>
       </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
       <c r="G61" t="s">
         <v>9</v>
       </c>
@@ -2157,12 +2043,6 @@
         <v>1</v>
       </c>
       <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="F62">
         <v>0</v>
       </c>
       <c r="G62" t="s">
@@ -2185,12 +2065,6 @@
       <c r="D63">
         <v>24</v>
       </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
       <c r="G63" t="s">
         <v>9</v>
       </c>
@@ -2212,9 +2086,6 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>0</v>
-      </c>
-      <c r="F64">
         <v>0</v>
       </c>
       <c r="G64" t="s">
@@ -2422,9 +2293,6 @@
       <c r="E72">
         <v>0</v>
       </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
       <c r="G72" t="s">
         <v>9</v>
       </c>
@@ -2448,9 +2316,6 @@
       <c r="E73">
         <v>0</v>
       </c>
-      <c r="F73">
-        <v>0</v>
-      </c>
       <c r="G73" t="s">
         <v>9</v>
       </c>
@@ -2524,9 +2389,6 @@
         <v>0</v>
       </c>
       <c r="E76">
-        <v>0</v>
-      </c>
-      <c r="F76">
         <v>0</v>
       </c>
       <c r="G76" t="s">
@@ -2578,9 +2440,6 @@
       <c r="E78">
         <v>1</v>
       </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
       <c r="G78" t="s">
         <v>9</v>
       </c>
@@ -2682,9 +2541,6 @@
       <c r="E82">
         <v>0</v>
       </c>
-      <c r="F82">
-        <v>0</v>
-      </c>
       <c r="G82" t="s">
         <v>9</v>
       </c>
@@ -2705,12 +2561,6 @@
       <c r="D83">
         <v>5</v>
       </c>
-      <c r="E83">
-        <v>0</v>
-      </c>
-      <c r="F83">
-        <v>0</v>
-      </c>
       <c r="G83" t="s">
         <v>9</v>
       </c>
@@ -2730,12 +2580,6 @@
       </c>
       <c r="D84">
         <v>9</v>
-      </c>
-      <c r="E84">
-        <v>0</v>
-      </c>
-      <c r="F84">
-        <v>0</v>
       </c>
       <c r="G84" t="s">
         <v>9</v>
@@ -2786,9 +2630,6 @@
       <c r="E86">
         <v>0</v>
       </c>
-      <c r="F86">
-        <v>0</v>
-      </c>
       <c r="G86" t="s">
         <v>9</v>
       </c>
@@ -2838,9 +2679,6 @@
       <c r="E88">
         <v>0</v>
       </c>
-      <c r="F88">
-        <v>0</v>
-      </c>
       <c r="G88" t="s">
         <v>9</v>
       </c>
@@ -2859,12 +2697,6 @@
         <v>0</v>
       </c>
       <c r="D89">
-        <v>0</v>
-      </c>
-      <c r="E89">
-        <v>0</v>
-      </c>
-      <c r="F89">
         <v>0</v>
       </c>
       <c r="G89" t="s">
@@ -2916,9 +2748,6 @@
       <c r="E91">
         <v>1455</v>
       </c>
-      <c r="F91">
-        <v>0</v>
-      </c>
       <c r="G91" t="s">
         <v>10</v>
       </c>
@@ -3020,9 +2849,6 @@
       <c r="E95">
         <v>0</v>
       </c>
-      <c r="F95">
-        <v>0</v>
-      </c>
       <c r="G95" t="s">
         <v>10</v>
       </c>
@@ -3041,12 +2867,6 @@
         <v>0</v>
       </c>
       <c r="D96">
-        <v>0</v>
-      </c>
-      <c r="E96">
-        <v>0</v>
-      </c>
-      <c r="F96">
         <v>0</v>
       </c>
       <c r="G96" t="s">
@@ -3098,9 +2918,6 @@
       <c r="E98">
         <v>44</v>
       </c>
-      <c r="F98">
-        <v>0</v>
-      </c>
       <c r="G98" t="s">
         <v>10</v>
       </c>
@@ -3150,9 +2967,6 @@
       <c r="E100">
         <v>23</v>
       </c>
-      <c r="F100">
-        <v>0</v>
-      </c>
       <c r="G100" t="s">
         <v>10</v>
       </c>
@@ -3176,9 +2990,6 @@
       <c r="E101">
         <v>38</v>
       </c>
-      <c r="F101">
-        <v>0</v>
-      </c>
       <c r="G101" t="s">
         <v>10</v>
       </c>
@@ -3228,9 +3039,6 @@
       <c r="E103">
         <v>139</v>
       </c>
-      <c r="F103">
-        <v>0</v>
-      </c>
       <c r="G103" t="s">
         <v>10</v>
       </c>
@@ -3254,9 +3062,6 @@
       <c r="E104">
         <v>4658</v>
       </c>
-      <c r="F104">
-        <v>0</v>
-      </c>
       <c r="G104" t="s">
         <v>10</v>
       </c>
@@ -3280,9 +3085,6 @@
       <c r="E105">
         <v>0</v>
       </c>
-      <c r="F105">
-        <v>0</v>
-      </c>
       <c r="G105" t="s">
         <v>10</v>
       </c>
@@ -3302,12 +3104,6 @@
       </c>
       <c r="D106">
         <v>7</v>
-      </c>
-      <c r="E106">
-        <v>0</v>
-      </c>
-      <c r="F106">
-        <v>0</v>
       </c>
       <c r="G106" t="s">
         <v>10</v>
@@ -3329,12 +3125,6 @@
       <c r="D107">
         <v>244</v>
       </c>
-      <c r="E107">
-        <v>0</v>
-      </c>
-      <c r="F107">
-        <v>0</v>
-      </c>
       <c r="G107" t="s">
         <v>10</v>
       </c>
@@ -3356,9 +3146,6 @@
         <v>0</v>
       </c>
       <c r="E108">
-        <v>0</v>
-      </c>
-      <c r="F108">
         <v>0</v>
       </c>
       <c r="G108" t="s">
@@ -3566,9 +3353,6 @@
       <c r="E116">
         <v>1</v>
       </c>
-      <c r="F116">
-        <v>0</v>
-      </c>
       <c r="G116" t="s">
         <v>10</v>
       </c>
@@ -3590,9 +3374,6 @@
         <v>1</v>
       </c>
       <c r="E117">
-        <v>0</v>
-      </c>
-      <c r="F117">
         <v>0</v>
       </c>
       <c r="G117" t="s">
@@ -3670,9 +3451,6 @@
       <c r="E120">
         <v>6</v>
       </c>
-      <c r="F120">
-        <v>0</v>
-      </c>
       <c r="G120" t="s">
         <v>10</v>
       </c>
@@ -3720,9 +3498,6 @@
         <v>1</v>
       </c>
       <c r="E122">
-        <v>0</v>
-      </c>
-      <c r="F122">
         <v>0</v>
       </c>
       <c r="G122" t="s">
@@ -3826,9 +3601,6 @@
       <c r="E126">
         <v>2851</v>
       </c>
-      <c r="F126">
-        <v>0</v>
-      </c>
       <c r="G126" t="s">
         <v>10</v>
       </c>
@@ -3849,12 +3621,6 @@
       <c r="D127">
         <v>118</v>
       </c>
-      <c r="E127">
-        <v>0</v>
-      </c>
-      <c r="F127">
-        <v>0</v>
-      </c>
       <c r="G127" t="s">
         <v>10</v>
       </c>
@@ -3875,12 +3641,6 @@
       <c r="D128">
         <v>17</v>
       </c>
-      <c r="E128">
-        <v>0</v>
-      </c>
-      <c r="F128">
-        <v>0</v>
-      </c>
       <c r="G128" t="s">
         <v>10</v>
       </c>
@@ -3930,9 +3690,6 @@
       <c r="E130">
         <v>8</v>
       </c>
-      <c r="F130">
-        <v>0</v>
-      </c>
       <c r="G130" t="s">
         <v>10</v>
       </c>
@@ -3982,9 +3739,6 @@
       <c r="E132">
         <v>0</v>
       </c>
-      <c r="F132">
-        <v>0</v>
-      </c>
       <c r="G132" t="s">
         <v>10</v>
       </c>
@@ -4003,12 +3757,6 @@
         <v>0</v>
       </c>
       <c r="D133">
-        <v>0</v>
-      </c>
-      <c r="E133">
-        <v>0</v>
-      </c>
-      <c r="F133">
         <v>0</v>
       </c>
       <c r="G133" t="s">
@@ -4060,9 +3808,6 @@
       <c r="E135">
         <v>1026</v>
       </c>
-      <c r="F135">
-        <v>0</v>
-      </c>
       <c r="G135" t="s">
         <v>11</v>
       </c>
@@ -4164,9 +3909,6 @@
       <c r="E139">
         <v>0</v>
       </c>
-      <c r="F139">
-        <v>0</v>
-      </c>
       <c r="G139" t="s">
         <v>11</v>
       </c>
@@ -4187,12 +3929,6 @@
       <c r="D140">
         <v>0</v>
       </c>
-      <c r="E140">
-        <v>0</v>
-      </c>
-      <c r="F140">
-        <v>0</v>
-      </c>
       <c r="G140" t="s">
         <v>11</v>
       </c>
@@ -4242,9 +3978,6 @@
       <c r="E142">
         <v>14</v>
       </c>
-      <c r="F142">
-        <v>0</v>
-      </c>
       <c r="G142" t="s">
         <v>11</v>
       </c>
@@ -4294,9 +4027,6 @@
       <c r="E144">
         <v>113</v>
       </c>
-      <c r="F144">
-        <v>0</v>
-      </c>
       <c r="G144" t="s">
         <v>11</v>
       </c>
@@ -4320,9 +4050,6 @@
       <c r="E145">
         <v>150</v>
       </c>
-      <c r="F145">
-        <v>0</v>
-      </c>
       <c r="G145" t="s">
         <v>11</v>
       </c>
@@ -4372,9 +4099,6 @@
       <c r="E147">
         <v>26</v>
       </c>
-      <c r="F147">
-        <v>0</v>
-      </c>
       <c r="G147" t="s">
         <v>11</v>
       </c>
@@ -4398,9 +4122,6 @@
       <c r="E148">
         <v>727</v>
       </c>
-      <c r="F148">
-        <v>0</v>
-      </c>
       <c r="G148" t="s">
         <v>11</v>
       </c>
@@ -4424,9 +4145,6 @@
       <c r="E149">
         <v>0</v>
       </c>
-      <c r="F149">
-        <v>0</v>
-      </c>
       <c r="G149" t="s">
         <v>11</v>
       </c>
@@ -4446,12 +4164,6 @@
       </c>
       <c r="D150">
         <v>1</v>
-      </c>
-      <c r="E150">
-        <v>0</v>
-      </c>
-      <c r="F150">
-        <v>0</v>
       </c>
       <c r="G150" t="s">
         <v>11</v>
@@ -4473,12 +4185,6 @@
       <c r="D151">
         <v>20</v>
       </c>
-      <c r="E151">
-        <v>0</v>
-      </c>
-      <c r="F151">
-        <v>0</v>
-      </c>
       <c r="G151" t="s">
         <v>11</v>
       </c>
@@ -4501,9 +4207,6 @@
       </c>
       <c r="E152">
         <v>1</v>
-      </c>
-      <c r="F152">
-        <v>0</v>
       </c>
       <c r="G152" t="s">
         <v>11</v>
@@ -4710,9 +4413,6 @@
       <c r="E160">
         <v>0</v>
       </c>
-      <c r="F160">
-        <v>0</v>
-      </c>
       <c r="G160" t="s">
         <v>11</v>
       </c>
@@ -4735,9 +4435,6 @@
       </c>
       <c r="E161">
         <v>1</v>
-      </c>
-      <c r="F161">
-        <v>0</v>
       </c>
       <c r="G161" t="s">
         <v>11</v>
@@ -4814,9 +4511,6 @@
       <c r="E164">
         <v>1</v>
       </c>
-      <c r="F164">
-        <v>0</v>
-      </c>
       <c r="G164" t="s">
         <v>11</v>
       </c>
@@ -4866,9 +4560,6 @@
       <c r="E166">
         <v>24</v>
       </c>
-      <c r="F166">
-        <v>0</v>
-      </c>
       <c r="G166" t="s">
         <v>11</v>
       </c>
@@ -4970,9 +4661,6 @@
       <c r="E170">
         <v>3391</v>
       </c>
-      <c r="F170">
-        <v>0</v>
-      </c>
       <c r="G170" t="s">
         <v>11</v>
       </c>
@@ -4993,12 +4681,6 @@
       <c r="D171">
         <v>64</v>
       </c>
-      <c r="E171">
-        <v>0</v>
-      </c>
-      <c r="F171">
-        <v>0</v>
-      </c>
       <c r="G171" t="s">
         <v>11</v>
       </c>
@@ -5019,12 +4701,6 @@
       <c r="D172">
         <v>18</v>
       </c>
-      <c r="E172">
-        <v>0</v>
-      </c>
-      <c r="F172">
-        <v>0</v>
-      </c>
       <c r="G172" t="s">
         <v>11</v>
       </c>
@@ -5074,9 +4750,6 @@
       <c r="E174">
         <v>30</v>
       </c>
-      <c r="F174">
-        <v>0</v>
-      </c>
       <c r="G174" t="s">
         <v>11</v>
       </c>
@@ -5125,9 +4798,6 @@
       </c>
       <c r="E176">
         <v>1</v>
-      </c>
-      <c r="F176">
-        <v>0</v>
       </c>
       <c r="G176" t="s">
         <v>11</v>
@@ -5149,12 +4819,6 @@
       <c r="D177">
         <v>14</v>
       </c>
-      <c r="E177">
-        <v>0</v>
-      </c>
-      <c r="F177">
-        <v>0</v>
-      </c>
       <c r="G177" t="s">
         <v>11</v>
       </c>
@@ -5202,9 +4866,6 @@
         <v>0</v>
       </c>
       <c r="E179">
-        <v>0</v>
-      </c>
-      <c r="F179">
         <v>0</v>
       </c>
       <c r="G179" t="s">
@@ -5308,9 +4969,6 @@
       <c r="E183">
         <v>1</v>
       </c>
-      <c r="F183">
-        <v>0</v>
-      </c>
       <c r="G183" t="s">
         <v>12</v>
       </c>
@@ -5331,12 +4989,6 @@
       <c r="D184">
         <v>0</v>
       </c>
-      <c r="E184">
-        <v>0</v>
-      </c>
-      <c r="F184">
-        <v>0</v>
-      </c>
       <c r="G184" t="s">
         <v>12</v>
       </c>
@@ -5386,9 +5038,6 @@
       <c r="E186">
         <v>1</v>
       </c>
-      <c r="F186">
-        <v>0</v>
-      </c>
       <c r="G186" t="s">
         <v>12</v>
       </c>
@@ -5437,9 +5086,6 @@
       </c>
       <c r="E188">
         <v>25</v>
-      </c>
-      <c r="F188">
-        <v>0</v>
       </c>
       <c r="G188" t="s">
         <v>12</v>
@@ -5464,9 +5110,6 @@
       <c r="E189">
         <v>203</v>
       </c>
-      <c r="F189">
-        <v>0</v>
-      </c>
       <c r="G189" t="s">
         <v>12</v>
       </c>
@@ -5516,9 +5159,6 @@
       <c r="E191">
         <v>44</v>
       </c>
-      <c r="F191">
-        <v>0</v>
-      </c>
       <c r="G191" t="s">
         <v>12</v>
       </c>
@@ -5542,9 +5182,6 @@
       <c r="E192">
         <v>21</v>
       </c>
-      <c r="F192">
-        <v>0</v>
-      </c>
       <c r="G192" t="s">
         <v>12</v>
       </c>
@@ -5566,9 +5203,6 @@
         <v>5</v>
       </c>
       <c r="E193">
-        <v>0</v>
-      </c>
-      <c r="F193">
         <v>0</v>
       </c>
       <c r="G193" t="s">
@@ -5591,12 +5225,6 @@
       <c r="D194">
         <v>19</v>
       </c>
-      <c r="E194">
-        <v>0</v>
-      </c>
-      <c r="F194">
-        <v>0</v>
-      </c>
       <c r="G194" t="s">
         <v>12</v>
       </c>
@@ -5617,12 +5245,6 @@
       <c r="D195">
         <v>39</v>
       </c>
-      <c r="E195">
-        <v>0</v>
-      </c>
-      <c r="F195">
-        <v>0</v>
-      </c>
       <c r="G195" t="s">
         <v>12</v>
       </c>
@@ -5644,9 +5266,6 @@
         <v>0</v>
       </c>
       <c r="E196">
-        <v>0</v>
-      </c>
-      <c r="F196">
         <v>0</v>
       </c>
       <c r="G196" t="s">
@@ -5854,9 +5473,6 @@
       <c r="E204">
         <v>0</v>
       </c>
-      <c r="F204">
-        <v>0</v>
-      </c>
       <c r="G204" t="s">
         <v>12</v>
       </c>
@@ -5880,9 +5496,6 @@
       <c r="E205">
         <v>0</v>
       </c>
-      <c r="F205">
-        <v>0</v>
-      </c>
       <c r="G205" t="s">
         <v>12</v>
       </c>
@@ -5958,9 +5571,6 @@
       <c r="E208">
         <v>0</v>
       </c>
-      <c r="F208">
-        <v>0</v>
-      </c>
       <c r="G208" t="s">
         <v>12</v>
       </c>
@@ -6009,9 +5619,6 @@
       </c>
       <c r="E210">
         <v>1</v>
-      </c>
-      <c r="F210">
-        <v>0</v>
       </c>
       <c r="G210" t="s">
         <v>12</v>
@@ -6114,9 +5721,6 @@
       <c r="E214">
         <v>0</v>
       </c>
-      <c r="F214">
-        <v>0</v>
-      </c>
       <c r="G214" t="s">
         <v>12</v>
       </c>
@@ -6137,12 +5741,6 @@
       <c r="D215">
         <v>134</v>
       </c>
-      <c r="E215">
-        <v>0</v>
-      </c>
-      <c r="F215">
-        <v>0</v>
-      </c>
       <c r="G215" t="s">
         <v>12</v>
       </c>
@@ -6163,12 +5761,6 @@
       <c r="D216">
         <v>6</v>
       </c>
-      <c r="E216">
-        <v>0</v>
-      </c>
-      <c r="F216">
-        <v>0</v>
-      </c>
       <c r="G216" t="s">
         <v>12</v>
       </c>
@@ -6218,9 +5810,6 @@
       <c r="E218">
         <v>0</v>
       </c>
-      <c r="F218">
-        <v>0</v>
-      </c>
       <c r="G218" t="s">
         <v>12</v>
       </c>
@@ -6270,9 +5859,6 @@
       <c r="E220">
         <v>0</v>
       </c>
-      <c r="F220">
-        <v>0</v>
-      </c>
       <c r="G220" t="s">
         <v>12</v>
       </c>
@@ -6293,12 +5879,6 @@
       <c r="D221">
         <v>0</v>
       </c>
-      <c r="E221">
-        <v>0</v>
-      </c>
-      <c r="F221">
-        <v>0</v>
-      </c>
       <c r="G221" t="s">
         <v>12</v>
       </c>
@@ -6346,9 +5926,6 @@
         <v>0</v>
       </c>
       <c r="E223">
-        <v>0</v>
-      </c>
-      <c r="F223">
         <v>0</v>
       </c>
       <c r="G223" t="s">
@@ -6452,9 +6029,6 @@
       <c r="E227">
         <v>1</v>
       </c>
-      <c r="F227">
-        <v>0</v>
-      </c>
       <c r="G227" t="s">
         <v>13</v>
       </c>
@@ -6473,12 +6047,6 @@
         <v>0</v>
       </c>
       <c r="D228">
-        <v>0</v>
-      </c>
-      <c r="E228">
-        <v>0</v>
-      </c>
-      <c r="F228">
         <v>0</v>
       </c>
       <c r="G228" t="s">
@@ -6530,9 +6098,6 @@
       <c r="E230">
         <v>214</v>
       </c>
-      <c r="F230">
-        <v>0</v>
-      </c>
       <c r="G230" t="s">
         <v>13</v>
       </c>
@@ -6581,9 +6146,6 @@
       </c>
       <c r="E232">
         <v>1</v>
-      </c>
-      <c r="F232">
-        <v>0</v>
       </c>
       <c r="G232" t="s">
         <v>13</v>
@@ -6608,9 +6170,6 @@
       <c r="E233">
         <v>14</v>
       </c>
-      <c r="F233">
-        <v>0</v>
-      </c>
       <c r="G233" t="s">
         <v>13</v>
       </c>
@@ -6660,9 +6219,6 @@
       <c r="E235">
         <v>11</v>
       </c>
-      <c r="F235">
-        <v>0</v>
-      </c>
       <c r="G235" t="s">
         <v>13</v>
       </c>
@@ -6686,9 +6242,6 @@
       <c r="E236">
         <v>42</v>
       </c>
-      <c r="F236">
-        <v>0</v>
-      </c>
       <c r="G236" t="s">
         <v>13</v>
       </c>
@@ -6712,9 +6265,6 @@
       <c r="E237">
         <v>0</v>
       </c>
-      <c r="F237">
-        <v>0</v>
-      </c>
       <c r="G237" t="s">
         <v>13</v>
       </c>
@@ -6733,12 +6283,6 @@
         <v>0</v>
       </c>
       <c r="D238">
-        <v>0</v>
-      </c>
-      <c r="E238">
-        <v>0</v>
-      </c>
-      <c r="F238">
         <v>0</v>
       </c>
       <c r="G238" t="s">
@@ -6761,12 +6305,6 @@
       <c r="D239">
         <v>25</v>
       </c>
-      <c r="E239">
-        <v>0</v>
-      </c>
-      <c r="F239">
-        <v>0</v>
-      </c>
       <c r="G239" t="s">
         <v>13</v>
       </c>
@@ -6788,9 +6326,6 @@
         <v>0</v>
       </c>
       <c r="E240">
-        <v>0</v>
-      </c>
-      <c r="F240">
         <v>0</v>
       </c>
       <c r="G240" t="s">
@@ -6998,9 +6533,6 @@
       <c r="E248">
         <v>1</v>
       </c>
-      <c r="F248">
-        <v>0</v>
-      </c>
       <c r="G248" t="s">
         <v>13</v>
       </c>
@@ -7022,9 +6554,6 @@
         <v>0</v>
       </c>
       <c r="E249">
-        <v>0</v>
-      </c>
-      <c r="F249">
         <v>0</v>
       </c>
       <c r="G249" t="s">
@@ -7102,9 +6631,6 @@
       <c r="E252">
         <v>0</v>
       </c>
-      <c r="F252">
-        <v>0</v>
-      </c>
       <c r="G252" t="s">
         <v>13</v>
       </c>
@@ -7152,9 +6678,6 @@
         <v>0</v>
       </c>
       <c r="E254">
-        <v>0</v>
-      </c>
-      <c r="F254">
         <v>0</v>
       </c>
       <c r="G254" t="s">
@@ -7258,9 +6781,6 @@
       <c r="E258">
         <v>7</v>
       </c>
-      <c r="F258">
-        <v>0</v>
-      </c>
       <c r="G258" t="s">
         <v>13</v>
       </c>
@@ -7281,12 +6801,6 @@
       <c r="D259">
         <v>92</v>
       </c>
-      <c r="E259">
-        <v>0</v>
-      </c>
-      <c r="F259">
-        <v>0</v>
-      </c>
       <c r="G259" t="s">
         <v>13</v>
       </c>
@@ -7307,12 +6821,6 @@
       <c r="D260">
         <v>21</v>
       </c>
-      <c r="E260">
-        <v>0</v>
-      </c>
-      <c r="F260">
-        <v>0</v>
-      </c>
       <c r="G260" t="s">
         <v>13</v>
       </c>
@@ -7362,9 +6870,6 @@
       <c r="E262">
         <v>0</v>
       </c>
-      <c r="F262">
-        <v>0</v>
-      </c>
       <c r="G262" t="s">
         <v>13</v>
       </c>
@@ -7414,9 +6919,6 @@
       <c r="E264">
         <v>0</v>
       </c>
-      <c r="F264">
-        <v>0</v>
-      </c>
       <c r="G264" t="s">
         <v>13</v>
       </c>
@@ -7435,12 +6937,6 @@
         <v>0</v>
       </c>
       <c r="D265">
-        <v>0</v>
-      </c>
-      <c r="E265">
-        <v>0</v>
-      </c>
-      <c r="F265">
         <v>0</v>
       </c>
       <c r="G265" t="s">
@@ -7492,9 +6988,6 @@
       <c r="E267">
         <v>301</v>
       </c>
-      <c r="F267">
-        <v>0</v>
-      </c>
       <c r="G267" t="s">
         <v>14</v>
       </c>
@@ -7596,9 +7089,6 @@
       <c r="E271">
         <v>0</v>
       </c>
-      <c r="F271">
-        <v>0</v>
-      </c>
       <c r="G271" t="s">
         <v>14</v>
       </c>
@@ -7619,12 +7109,6 @@
       <c r="D272">
         <v>6</v>
       </c>
-      <c r="E272">
-        <v>0</v>
-      </c>
-      <c r="F272">
-        <v>0</v>
-      </c>
       <c r="G272" t="s">
         <v>14</v>
       </c>
@@ -7674,9 +7158,6 @@
       <c r="E274">
         <v>1</v>
       </c>
-      <c r="F274">
-        <v>0</v>
-      </c>
       <c r="G274" t="s">
         <v>14</v>
       </c>
@@ -7724,9 +7205,6 @@
         <v>1</v>
       </c>
       <c r="E276">
-        <v>0</v>
-      </c>
-      <c r="F276">
         <v>0</v>
       </c>
       <c r="G276" t="s">
@@ -7752,9 +7230,6 @@
       <c r="E277">
         <v>100</v>
       </c>
-      <c r="F277">
-        <v>0</v>
-      </c>
       <c r="G277" t="s">
         <v>14</v>
       </c>
@@ -7804,9 +7279,6 @@
       <c r="E279">
         <v>152</v>
       </c>
-      <c r="F279">
-        <v>0</v>
-      </c>
       <c r="G279" t="s">
         <v>14</v>
       </c>
@@ -7830,9 +7302,6 @@
       <c r="E280">
         <v>730</v>
       </c>
-      <c r="F280">
-        <v>0</v>
-      </c>
       <c r="G280" t="s">
         <v>14</v>
       </c>
@@ -7854,9 +7323,6 @@
         <v>0</v>
       </c>
       <c r="E281">
-        <v>0</v>
-      </c>
-      <c r="F281">
         <v>0</v>
       </c>
       <c r="G281" t="s">
@@ -7879,12 +7345,6 @@
       <c r="D282">
         <v>139</v>
       </c>
-      <c r="E282">
-        <v>0</v>
-      </c>
-      <c r="F282">
-        <v>0</v>
-      </c>
       <c r="G282" t="s">
         <v>14</v>
       </c>
@@ -7905,12 +7365,6 @@
       <c r="D283">
         <v>448</v>
       </c>
-      <c r="E283">
-        <v>0</v>
-      </c>
-      <c r="F283">
-        <v>0</v>
-      </c>
       <c r="G283" t="s">
         <v>14</v>
       </c>
@@ -7932,9 +7386,6 @@
         <v>0</v>
       </c>
       <c r="E284">
-        <v>0</v>
-      </c>
-      <c r="F284">
         <v>0</v>
       </c>
       <c r="G284" t="s">
@@ -8142,9 +7593,6 @@
       <c r="E292">
         <v>1</v>
       </c>
-      <c r="F292">
-        <v>0</v>
-      </c>
       <c r="G292" t="s">
         <v>14</v>
       </c>
@@ -8168,9 +7616,6 @@
       <c r="E293">
         <v>0</v>
       </c>
-      <c r="F293">
-        <v>0</v>
-      </c>
       <c r="G293" t="s">
         <v>14</v>
       </c>
@@ -8246,9 +7691,6 @@
       <c r="E296">
         <v>0</v>
       </c>
-      <c r="F296">
-        <v>0</v>
-      </c>
       <c r="G296" t="s">
         <v>14</v>
       </c>
@@ -8298,9 +7740,6 @@
       <c r="E298">
         <v>6</v>
       </c>
-      <c r="F298">
-        <v>0</v>
-      </c>
       <c r="G298" t="s">
         <v>14</v>
       </c>
@@ -8402,9 +7841,6 @@
       <c r="E302">
         <v>69</v>
       </c>
-      <c r="F302">
-        <v>0</v>
-      </c>
       <c r="G302" t="s">
         <v>14</v>
       </c>
@@ -8425,12 +7861,6 @@
       <c r="D303">
         <v>196</v>
       </c>
-      <c r="E303">
-        <v>0</v>
-      </c>
-      <c r="F303">
-        <v>0</v>
-      </c>
       <c r="G303" t="s">
         <v>14</v>
       </c>
@@ -8451,12 +7881,6 @@
       <c r="D304">
         <v>49</v>
       </c>
-      <c r="E304">
-        <v>0</v>
-      </c>
-      <c r="F304">
-        <v>0</v>
-      </c>
       <c r="G304" t="s">
         <v>14</v>
       </c>
@@ -8506,9 +7930,6 @@
       <c r="E306">
         <v>30</v>
       </c>
-      <c r="F306">
-        <v>0</v>
-      </c>
       <c r="G306" t="s">
         <v>14</v>
       </c>
@@ -8558,9 +7979,6 @@
       <c r="E308">
         <v>20</v>
       </c>
-      <c r="F308">
-        <v>0</v>
-      </c>
       <c r="G308" t="s">
         <v>14</v>
       </c>
@@ -8581,12 +7999,6 @@
       <c r="D309">
         <v>82</v>
       </c>
-      <c r="E309">
-        <v>0</v>
-      </c>
-      <c r="F309">
-        <v>0</v>
-      </c>
       <c r="G309" t="s">
         <v>14</v>
       </c>
@@ -8636,9 +8048,6 @@
       <c r="E311">
         <v>271</v>
       </c>
-      <c r="F311">
-        <v>0</v>
-      </c>
       <c r="G311" t="s">
         <v>15</v>
       </c>
@@ -8740,9 +8149,6 @@
       <c r="E315">
         <v>0</v>
       </c>
-      <c r="F315">
-        <v>0</v>
-      </c>
       <c r="G315" t="s">
         <v>15</v>
       </c>
@@ -8762,12 +8168,6 @@
       </c>
       <c r="D316">
         <v>6</v>
-      </c>
-      <c r="E316">
-        <v>0</v>
-      </c>
-      <c r="F316">
-        <v>0</v>
       </c>
       <c r="G316" t="s">
         <v>15</v>
@@ -8818,9 +8218,6 @@
       <c r="E318">
         <v>25</v>
       </c>
-      <c r="F318">
-        <v>0</v>
-      </c>
       <c r="G318" t="s">
         <v>15</v>
       </c>
@@ -8870,9 +8267,6 @@
       <c r="E320">
         <v>185</v>
       </c>
-      <c r="F320">
-        <v>0</v>
-      </c>
       <c r="G320" t="s">
         <v>15</v>
       </c>
@@ -8896,9 +8290,6 @@
       <c r="E321">
         <v>94</v>
       </c>
-      <c r="F321">
-        <v>0</v>
-      </c>
       <c r="G321" t="s">
         <v>15</v>
       </c>
@@ -8948,9 +8339,6 @@
       <c r="E323">
         <v>6</v>
       </c>
-      <c r="F323">
-        <v>0</v>
-      </c>
       <c r="G323" t="s">
         <v>15</v>
       </c>
@@ -8974,9 +8362,6 @@
       <c r="E324">
         <v>9</v>
       </c>
-      <c r="F324">
-        <v>0</v>
-      </c>
       <c r="G324" t="s">
         <v>15</v>
       </c>
@@ -9000,9 +8385,6 @@
       <c r="E325">
         <v>0</v>
       </c>
-      <c r="F325">
-        <v>0</v>
-      </c>
       <c r="G325" t="s">
         <v>15</v>
       </c>
@@ -9022,12 +8404,6 @@
       </c>
       <c r="D326">
         <v>1</v>
-      </c>
-      <c r="E326">
-        <v>0</v>
-      </c>
-      <c r="F326">
-        <v>0</v>
       </c>
       <c r="G326" t="s">
         <v>15</v>
@@ -9049,12 +8425,6 @@
       <c r="D327">
         <v>44</v>
       </c>
-      <c r="E327">
-        <v>0</v>
-      </c>
-      <c r="F327">
-        <v>0</v>
-      </c>
       <c r="G327" t="s">
         <v>15</v>
       </c>
@@ -9076,9 +8446,6 @@
         <v>0</v>
       </c>
       <c r="E328">
-        <v>0</v>
-      </c>
-      <c r="F328">
         <v>0</v>
       </c>
       <c r="G328" t="s">
@@ -9390,9 +8757,6 @@
       <c r="E340">
         <v>0</v>
       </c>
-      <c r="F340">
-        <v>0</v>
-      </c>
       <c r="G340" t="s">
         <v>15</v>
       </c>
@@ -9442,9 +8806,6 @@
       <c r="E342">
         <v>5</v>
       </c>
-      <c r="F342">
-        <v>0</v>
-      </c>
       <c r="G342" t="s">
         <v>15</v>
       </c>
@@ -9546,9 +8907,6 @@
       <c r="E346">
         <v>31</v>
       </c>
-      <c r="F346">
-        <v>0</v>
-      </c>
       <c r="G346" t="s">
         <v>15</v>
       </c>
@@ -9569,12 +8927,6 @@
       <c r="D347">
         <v>34</v>
       </c>
-      <c r="E347">
-        <v>0</v>
-      </c>
-      <c r="F347">
-        <v>0</v>
-      </c>
       <c r="G347" t="s">
         <v>15</v>
       </c>
@@ -9595,12 +8947,6 @@
       <c r="D348">
         <v>28</v>
       </c>
-      <c r="E348">
-        <v>0</v>
-      </c>
-      <c r="F348">
-        <v>0</v>
-      </c>
       <c r="G348" t="s">
         <v>15</v>
       </c>
@@ -9650,9 +8996,6 @@
       <c r="E350">
         <v>1</v>
       </c>
-      <c r="F350">
-        <v>0</v>
-      </c>
       <c r="G350" t="s">
         <v>15</v>
       </c>
@@ -9702,9 +9045,6 @@
       <c r="E352">
         <v>0</v>
       </c>
-      <c r="F352">
-        <v>0</v>
-      </c>
       <c r="G352" t="s">
         <v>15</v>
       </c>
@@ -9725,12 +9065,6 @@
       <c r="D353">
         <v>0</v>
       </c>
-      <c r="E353">
-        <v>0</v>
-      </c>
-      <c r="F353">
-        <v>0</v>
-      </c>
       <c r="G353" t="s">
         <v>15</v>
       </c>
@@ -9778,9 +9112,6 @@
         <v>0</v>
       </c>
       <c r="E355">
-        <v>0</v>
-      </c>
-      <c r="F355">
         <v>0</v>
       </c>
       <c r="G355" t="s">
@@ -9884,9 +9215,6 @@
       <c r="E359">
         <v>0</v>
       </c>
-      <c r="F359">
-        <v>0</v>
-      </c>
       <c r="G359" t="s">
         <v>16</v>
       </c>
@@ -9905,12 +9233,6 @@
         <v>0</v>
       </c>
       <c r="D360">
-        <v>0</v>
-      </c>
-      <c r="E360">
-        <v>0</v>
-      </c>
-      <c r="F360">
         <v>0</v>
       </c>
       <c r="G360" t="s">
@@ -9962,9 +9284,6 @@
       <c r="E362">
         <v>5</v>
       </c>
-      <c r="F362">
-        <v>0</v>
-      </c>
       <c r="G362" t="s">
         <v>16</v>
       </c>
@@ -10012,9 +9331,6 @@
         <v>1</v>
       </c>
       <c r="E364">
-        <v>0</v>
-      </c>
-      <c r="F364">
         <v>0</v>
       </c>
       <c r="G364" t="s">
@@ -10040,9 +9356,6 @@
       <c r="E365">
         <v>237</v>
       </c>
-      <c r="F365">
-        <v>0</v>
-      </c>
       <c r="G365" t="s">
         <v>16</v>
       </c>
@@ -10092,9 +9405,6 @@
       <c r="E367">
         <v>7</v>
       </c>
-      <c r="F367">
-        <v>0</v>
-      </c>
       <c r="G367" t="s">
         <v>16</v>
       </c>
@@ -10118,9 +9428,6 @@
       <c r="E368">
         <v>0</v>
       </c>
-      <c r="F368">
-        <v>0</v>
-      </c>
       <c r="G368" t="s">
         <v>16</v>
       </c>
@@ -10144,9 +9451,6 @@
       <c r="E369">
         <v>0</v>
       </c>
-      <c r="F369">
-        <v>0</v>
-      </c>
       <c r="G369" t="s">
         <v>16</v>
       </c>
@@ -10165,12 +9469,6 @@
         <v>1</v>
       </c>
       <c r="D370">
-        <v>0</v>
-      </c>
-      <c r="E370">
-        <v>0</v>
-      </c>
-      <c r="F370">
         <v>0</v>
       </c>
       <c r="G370" t="s">
@@ -10193,12 +9491,6 @@
       <c r="D371">
         <v>19</v>
       </c>
-      <c r="E371">
-        <v>0</v>
-      </c>
-      <c r="F371">
-        <v>0</v>
-      </c>
       <c r="G371" t="s">
         <v>16</v>
       </c>
@@ -10220,9 +9512,6 @@
         <v>0</v>
       </c>
       <c r="E372">
-        <v>0</v>
-      </c>
-      <c r="F372">
         <v>0</v>
       </c>
       <c r="G372" t="s">
@@ -10430,9 +9719,6 @@
       <c r="E380">
         <v>0</v>
       </c>
-      <c r="F380">
-        <v>0</v>
-      </c>
       <c r="G380" t="s">
         <v>16</v>
       </c>
@@ -10456,9 +9742,6 @@
       <c r="E381">
         <v>1</v>
       </c>
-      <c r="F381">
-        <v>0</v>
-      </c>
       <c r="G381" t="s">
         <v>16</v>
       </c>
@@ -10532,9 +9815,6 @@
         <v>0</v>
       </c>
       <c r="E384">
-        <v>0</v>
-      </c>
-      <c r="F384">
         <v>0</v>
       </c>
       <c r="G384" t="s">
@@ -10586,9 +9866,6 @@
       <c r="E386">
         <v>11</v>
       </c>
-      <c r="F386">
-        <v>0</v>
-      </c>
       <c r="G386" t="s">
         <v>16</v>
       </c>
@@ -10690,9 +9967,6 @@
       <c r="E390">
         <v>0</v>
       </c>
-      <c r="F390">
-        <v>0</v>
-      </c>
       <c r="G390" t="s">
         <v>16</v>
       </c>
@@ -10713,12 +9987,6 @@
       <c r="D391">
         <v>35</v>
       </c>
-      <c r="E391">
-        <v>0</v>
-      </c>
-      <c r="F391">
-        <v>0</v>
-      </c>
       <c r="G391" t="s">
         <v>16</v>
       </c>
@@ -10739,12 +10007,6 @@
       <c r="D392">
         <v>151</v>
       </c>
-      <c r="E392">
-        <v>0</v>
-      </c>
-      <c r="F392">
-        <v>0</v>
-      </c>
       <c r="G392" t="s">
         <v>16</v>
       </c>
@@ -10794,9 +10056,6 @@
       <c r="E394">
         <v>123</v>
       </c>
-      <c r="F394">
-        <v>0</v>
-      </c>
       <c r="G394" t="s">
         <v>16</v>
       </c>
@@ -10845,9 +10104,6 @@
       </c>
       <c r="E396">
         <v>39</v>
-      </c>
-      <c r="F396">
-        <v>0</v>
       </c>
       <c r="G396" t="s">
         <v>16</v>
@@ -10869,12 +10125,6 @@
       <c r="D397">
         <v>12</v>
       </c>
-      <c r="E397">
-        <v>0</v>
-      </c>
-      <c r="F397">
-        <v>0</v>
-      </c>
       <c r="G397" t="s">
         <v>16</v>
       </c>
@@ -10924,9 +10174,6 @@
       <c r="E399">
         <v>40</v>
       </c>
-      <c r="F399">
-        <v>0</v>
-      </c>
       <c r="G399" t="s">
         <v>17</v>
       </c>
@@ -11028,9 +10275,6 @@
       <c r="E403">
         <v>1</v>
       </c>
-      <c r="F403">
-        <v>0</v>
-      </c>
       <c r="G403" t="s">
         <v>17</v>
       </c>
@@ -11050,12 +10294,6 @@
       </c>
       <c r="D404">
         <v>11</v>
-      </c>
-      <c r="E404">
-        <v>0</v>
-      </c>
-      <c r="F404">
-        <v>0</v>
       </c>
       <c r="G404" t="s">
         <v>17</v>
@@ -11106,9 +10344,6 @@
       <c r="E406">
         <v>5</v>
       </c>
-      <c r="F406">
-        <v>0</v>
-      </c>
       <c r="G406" t="s">
         <v>17</v>
       </c>
@@ -11157,9 +10392,6 @@
       </c>
       <c r="E408">
         <v>1</v>
-      </c>
-      <c r="F408">
-        <v>0</v>
       </c>
       <c r="G408" t="s">
         <v>17</v>
@@ -11184,9 +10416,6 @@
       <c r="E409">
         <v>122</v>
       </c>
-      <c r="F409">
-        <v>0</v>
-      </c>
       <c r="G409" t="s">
         <v>17</v>
       </c>
@@ -11236,9 +10465,6 @@
       <c r="E411">
         <v>18</v>
       </c>
-      <c r="F411">
-        <v>0</v>
-      </c>
       <c r="G411" t="s">
         <v>17</v>
       </c>
@@ -11262,9 +10488,6 @@
       <c r="E412">
         <v>5</v>
       </c>
-      <c r="F412">
-        <v>0</v>
-      </c>
       <c r="G412" t="s">
         <v>17</v>
       </c>
@@ -11286,9 +10509,6 @@
         <v>0</v>
       </c>
       <c r="E413">
-        <v>0</v>
-      </c>
-      <c r="F413">
         <v>0</v>
       </c>
       <c r="G413" t="s">
@@ -11311,12 +10531,6 @@
       <c r="D414">
         <v>0</v>
       </c>
-      <c r="E414">
-        <v>0</v>
-      </c>
-      <c r="F414">
-        <v>0</v>
-      </c>
       <c r="G414" t="s">
         <v>17</v>
       </c>
@@ -11337,12 +10551,6 @@
       <c r="D415">
         <v>540</v>
       </c>
-      <c r="E415">
-        <v>0</v>
-      </c>
-      <c r="F415">
-        <v>0</v>
-      </c>
       <c r="G415" t="s">
         <v>17</v>
       </c>
@@ -11366,9 +10574,6 @@
       <c r="E416">
         <v>1</v>
       </c>
-      <c r="F416">
-        <v>0</v>
-      </c>
       <c r="G416" t="s">
         <v>17</v>
       </c>
@@ -11574,9 +10779,6 @@
       <c r="E424">
         <v>103</v>
       </c>
-      <c r="F424">
-        <v>0</v>
-      </c>
       <c r="G424" t="s">
         <v>17</v>
       </c>
@@ -11600,9 +10802,6 @@
       <c r="E425">
         <v>38</v>
       </c>
-      <c r="F425">
-        <v>0</v>
-      </c>
       <c r="G425" t="s">
         <v>17</v>
       </c>
@@ -11677,9 +10876,6 @@
       </c>
       <c r="E428">
         <v>1</v>
-      </c>
-      <c r="F428">
-        <v>0</v>
       </c>
       <c r="G428" t="s">
         <v>17</v>
@@ -11730,9 +10926,6 @@
       <c r="E430">
         <v>28</v>
       </c>
-      <c r="F430">
-        <v>0</v>
-      </c>
       <c r="G430" t="s">
         <v>17</v>
       </c>
@@ -11834,9 +11027,6 @@
       <c r="E434">
         <v>0</v>
       </c>
-      <c r="F434">
-        <v>0</v>
-      </c>
       <c r="G434" t="s">
         <v>17</v>
       </c>
@@ -11857,12 +11047,6 @@
       <c r="D435">
         <v>39</v>
       </c>
-      <c r="E435">
-        <v>0</v>
-      </c>
-      <c r="F435">
-        <v>0</v>
-      </c>
       <c r="G435" t="s">
         <v>17</v>
       </c>
@@ -11883,12 +11067,6 @@
       <c r="D436">
         <v>36</v>
       </c>
-      <c r="E436">
-        <v>0</v>
-      </c>
-      <c r="F436">
-        <v>0</v>
-      </c>
       <c r="G436" t="s">
         <v>17</v>
       </c>
@@ -11938,9 +11116,6 @@
       <c r="E438">
         <v>1</v>
       </c>
-      <c r="F438">
-        <v>0</v>
-      </c>
       <c r="G438" t="s">
         <v>17</v>
       </c>
@@ -11990,9 +11165,6 @@
       <c r="E440">
         <v>0</v>
       </c>
-      <c r="F440">
-        <v>0</v>
-      </c>
       <c r="G440" t="s">
         <v>17</v>
       </c>
@@ -12011,12 +11183,6 @@
         <v>1</v>
       </c>
       <c r="D441">
-        <v>0</v>
-      </c>
-      <c r="E441">
-        <v>0</v>
-      </c>
-      <c r="F441">
         <v>0</v>
       </c>
       <c r="G441" t="s">

</xml_diff>